<commit_message>
Updated Albert's Computer Folders
</commit_message>
<xml_diff>
--- a/ComputerFolders.xlsx
+++ b/ComputerFolders.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="19440" windowHeight="12240"/>
+    <workbookView xWindow="120" yWindow="48" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
   <si>
     <t>Computer Name</t>
   </si>
@@ -57,12 +57,6 @@
     <t>albert-pc</t>
   </si>
   <si>
-    <t>C:\Users\Albert\Documents\Princeton\Gregor Lab\Data Analysis\LivemRNA\Analysis\MS2\MCPNoNLS+MS2</t>
-  </si>
-  <si>
-    <t>C:\Users\Albert\Documents\Princeton\Gregor Lab\Data Analysis\FISHDrosophila</t>
-  </si>
-  <si>
     <t>C:\Users\Albert\Dropbox\LivemRNAData</t>
   </si>
   <si>
@@ -127,6 +121,15 @@
   </si>
   <si>
     <t>C:\Users\hgarcia\Documents\My Papers\LivemRNA\mRNADynamics</t>
+  </si>
+  <si>
+    <t>C:\Users\Albert\Documents\Princeton\Gregor Lab\Data Analysis\LivemRNA\RawData</t>
+  </si>
+  <si>
+    <t>C:\Users\Albert\Documents\Princeton\Gregor Lab\Data Analysis\LivemRNA\FISHAnalysisData</t>
+  </si>
+  <si>
+    <t>C:\Users\Albert\Documents\Princeton\Gregor Lab\Data Analysis\LivemRNA\mRNADynamics</t>
   </si>
 </sst>
 </file>
@@ -476,21 +479,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="76.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="99.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="99.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -504,16 +507,16 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -521,22 +524,22 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -544,90 +547,93 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="s">
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
         <v>33</v>
       </c>
-      <c r="G6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -638,13 +644,13 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -659,7 +665,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -671,7 +677,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added esmith10laptop to ComputerFolders
Also, first attempt to merge EricDev with master
</commit_message>
<xml_diff>
--- a/ComputerFolders.xlsx
+++ b/ComputerFolders.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\E\GitHub\mRNADynamics\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="48" windowWidth="19440" windowHeight="12240"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>Computer Name</t>
   </si>
@@ -130,6 +135,18 @@
   </si>
   <si>
     <t>C:\Users\Albert\Documents\Princeton\Gregor Lab\Data Analysis\LivemRNA\mRNADynamics</t>
+  </si>
+  <si>
+    <t>esmith10laptop</t>
+  </si>
+  <si>
+    <t>C:\E\Local\Lab\[07] Transcription\RawData</t>
+  </si>
+  <si>
+    <t>C:\E\Local\Lab\[07] Transcription\FISHAnalysisData</t>
+  </si>
+  <si>
+    <t>C:\E\SkyDrive\Lab\[07] Transcription\LivemRNAData</t>
   </si>
 </sst>
 </file>
@@ -186,6 +203,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -233,7 +253,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -268,7 +288,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -477,23 +497,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2040" topLeftCell="G1" activePane="topRight"/>
+      <selection pane="topRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="76.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="99.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="99.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="47.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,8 +538,11 @@
       <c r="G1" t="s">
         <v>21</v>
       </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -538,8 +564,11 @@
       <c r="G2" t="s">
         <v>27</v>
       </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -561,8 +590,11 @@
       <c r="G3" t="s">
         <v>28</v>
       </c>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -584,8 +616,11 @@
       <c r="G4" t="s">
         <v>20</v>
       </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -608,7 +643,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -619,7 +654,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -633,7 +668,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -665,7 +700,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -677,7 +712,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding MS2 code entry for esmith10laptop
</commit_message>
<xml_diff>
--- a/ComputerFolders.xlsx
+++ b/ComputerFolders.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t>Computer Name</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>C:\E\SkyDrive\Lab\[07] Transcription\LivemRNAData</t>
+  </si>
+  <si>
+    <t>C:\E\GitHub\mRNADynamics</t>
   </si>
 </sst>
 </file>
@@ -500,8 +503,8 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2040" topLeftCell="G1" activePane="topRight"/>
-      <selection pane="topRight" activeCell="H5" sqref="H5"/>
+      <pane xSplit="2040" topLeftCell="F1" activePane="topRight"/>
+      <selection pane="topRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,6 +669,9 @@
       </c>
       <c r="G7" t="s">
         <v>33</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added my folders to excel file as test.
Signed-off-by: Jacques Bothma Desktop <jpbothma@gmail.com>
</commit_message>
<xml_diff>
--- a/ComputerFolders.xlsx
+++ b/ComputerFolders.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\E\GitHub\mRNADynamics\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>Computer Name</t>
   </si>
@@ -150,6 +145,24 @@
   </si>
   <si>
     <t>C:\E\GitHub\mRNADynamics</t>
+  </si>
+  <si>
+    <t>bothma-desktop</t>
+  </si>
+  <si>
+    <t>D:\MS2LiveImaging\SourcePath</t>
+  </si>
+  <si>
+    <t>D:\MS2LiveImaging\Code\MS2Pausing\FISHCode</t>
+  </si>
+  <si>
+    <t>C:\Users\bothma\Dropbox\MS2Pausing</t>
+  </si>
+  <si>
+    <t>D:\MS2LiveImaging\Code\MS2Pausing\MS2Code</t>
+  </si>
+  <si>
+    <t>D:\MS2LiveImaging\SchnitzcellsFolder</t>
   </si>
 </sst>
 </file>
@@ -256,7 +269,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -291,7 +304,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -500,11 +513,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2040" topLeftCell="F1" activePane="topRight"/>
-      <selection pane="topRight" activeCell="I7" sqref="I7"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,7 +532,7 @@
     <col min="8" max="8" width="47.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,8 +557,11 @@
       <c r="H1" t="s">
         <v>38</v>
       </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -570,8 +586,11 @@
       <c r="H2" t="s">
         <v>39</v>
       </c>
+      <c r="I2" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -596,8 +615,11 @@
       <c r="H3" t="s">
         <v>40</v>
       </c>
+      <c r="I3" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -622,8 +644,11 @@
       <c r="H4" t="s">
         <v>41</v>
       </c>
+      <c r="I4" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -646,7 +671,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -656,8 +681,11 @@
       <c r="G6" t="s">
         <v>30</v>
       </c>
+      <c r="I6" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -673,8 +701,11 @@
       <c r="H7" t="s">
         <v>42</v>
       </c>
+      <c r="I7" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -692,6 +723,9 @@
       </c>
       <c r="G8" t="s">
         <v>22</v>
+      </c>
+      <c r="I8" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding support for multiple users on a computer
In order for both Hernan and Eric to be able to analyze data on
phy-tglab11, using different folders
</commit_message>
<xml_diff>
--- a/ComputerFolders.xlsx
+++ b/ComputerFolders.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\E\GitHub\mRNADynamics\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
   <si>
     <t>Computer Name</t>
   </si>
@@ -163,6 +168,27 @@
   </si>
   <si>
     <t>D:\MS2LiveImaging\SchnitzcellsFolder</t>
+  </si>
+  <si>
+    <t>User Name</t>
+  </si>
+  <si>
+    <t>hgarcia</t>
+  </si>
+  <si>
+    <t>emsthree</t>
+  </si>
+  <si>
+    <t>F:\Eric\Local\[07] Transcription\RawData</t>
+  </si>
+  <si>
+    <t>F:\Eric\Local\[07] Transcription\FISHAnalysisData</t>
+  </si>
+  <si>
+    <t>F:\Eric\Dropbox\LivemRNAData</t>
+  </si>
+  <si>
+    <t>F:\Eric\GitHub\mRNADynamics</t>
   </si>
 </sst>
 </file>
@@ -269,7 +295,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -304,7 +330,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -513,11 +539,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2040" topLeftCell="F1" activePane="topRight"/>
-      <selection pane="topRight" activeCell="I1" sqref="I1:I8"/>
+      <pane xSplit="2040" topLeftCell="G1" activePane="topRight"/>
+      <selection activeCell="A2" sqref="A2"/>
+      <selection pane="topRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,10 +556,11 @@
     <col min="5" max="5" width="49.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="39" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -555,102 +583,93 @@
         <v>21</v>
       </c>
       <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G3" t="s">
         <v>27</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" t="s">
         <v>39</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>36</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>28</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" t="s">
         <v>40</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>32</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
@@ -670,61 +689,96 @@
       <c r="G5" t="s">
         <v>20</v>
       </c>
+      <c r="H5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>31</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" t="s">
         <v>30</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>34</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>37</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G8" t="s">
         <v>33</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H8" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" t="s">
         <v>42</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>18</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>22</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G9" t="s">
         <v>22</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J9" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modifying esmith10laptop's Dropbox folder
</commit_message>
<xml_diff>
--- a/ComputerFolders.xlsx
+++ b/ComputerFolders.xlsx
@@ -146,9 +146,6 @@
     <t>C:\E\Local\Lab\[07] Transcription\FISHAnalysisData</t>
   </si>
   <si>
-    <t>C:\E\SkyDrive\Lab\[07] Transcription\LivemRNAData</t>
-  </si>
-  <si>
     <t>C:\E\GitHub\mRNADynamics</t>
   </si>
   <si>
@@ -189,6 +186,9 @@
   </si>
   <si>
     <t>F:\Eric\GitHub\mRNADynamics</t>
+  </si>
+  <si>
+    <t>C:\E\Dropbox\LivemRNAData</t>
   </si>
 </sst>
 </file>
@@ -542,9 +542,9 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2040" topLeftCell="G1" activePane="topRight"/>
+      <pane xSplit="2040" topLeftCell="H1" activePane="topRight"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="H2" sqref="H2"/>
+      <selection pane="topRight" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,18 +589,18 @@
         <v>38</v>
       </c>
       <c r="J1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" t="s">
         <v>49</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>50</v>
-      </c>
-      <c r="H2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -626,13 +626,13 @@
         <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I3" t="s">
         <v>39</v>
       </c>
       <c r="J3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -658,13 +658,13 @@
         <v>28</v>
       </c>
       <c r="H4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I4" t="s">
         <v>40</v>
       </c>
       <c r="J4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -690,13 +690,13 @@
         <v>20</v>
       </c>
       <c r="H5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I5" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="J5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -733,7 +733,7 @@
         <v>30</v>
       </c>
       <c r="J7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -750,13 +750,13 @@
         <v>33</v>
       </c>
       <c r="H8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -779,7 +779,7 @@
         <v>22</v>
       </c>
       <c r="J9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Jacques' Laptop to Computers to look for.
</commit_message>
<xml_diff>
--- a/ComputerFolders.xlsx
+++ b/ComputerFolders.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\E\GitHub\mRNADynamics\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="19440" windowHeight="12240"/>
+    <workbookView xWindow="120" yWindow="40" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="60">
   <si>
     <t>Computer Name</t>
   </si>
@@ -189,13 +189,25 @@
   </si>
   <si>
     <t>C:\E\Dropbox\LivemRNAData</t>
+  </si>
+  <si>
+    <t>jacquess-macbook-pro.local</t>
+  </si>
+  <si>
+    <t>/Users/bothma/FISHAnalysisData</t>
+  </si>
+  <si>
+    <t>/Users/bothma/Dropbox/MS2Pausing</t>
+  </si>
+  <si>
+    <t>/Users/bothma/mRNADynamics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +219,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -232,9 +251,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -295,7 +315,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -330,7 +350,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -539,28 +559,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2040" topLeftCell="H1" activePane="topRight"/>
+      <pane xSplit="4720" topLeftCell="J1" activePane="topRight"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="I5" sqref="I5"/>
+      <selection pane="topRight" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="76.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="99.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="99.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="39" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="50.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -591,8 +612,11 @@
       <c r="J1" t="s">
         <v>42</v>
       </c>
+      <c r="K1" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
@@ -602,8 +626,9 @@
       <c r="H2" t="s">
         <v>50</v>
       </c>
+      <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -635,7 +660,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -666,8 +691,11 @@
       <c r="J4" t="s">
         <v>44</v>
       </c>
+      <c r="K4" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -698,8 +726,11 @@
       <c r="J5" t="s">
         <v>45</v>
       </c>
+      <c r="K5" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -722,7 +753,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -735,8 +766,11 @@
       <c r="J7" t="s">
         <v>45</v>
       </c>
+      <c r="K7" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -758,8 +792,11 @@
       <c r="J8" t="s">
         <v>46</v>
       </c>
+      <c r="K8" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -784,7 +821,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -794,9 +836,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -806,8 +853,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New entry in ComputerFolders
</commit_message>
<xml_diff>
--- a/ComputerFolders.xlsx
+++ b/ComputerFolders.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\E\GitHub\Lab\mRNADynamics\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
   <si>
     <t>Computer Name</t>
   </si>
@@ -201,6 +206,15 @@
   </si>
   <si>
     <t>C:\Users\bothma\Documents\MATLAB\MS2CodeGit\mRNADynamics</t>
+  </si>
+  <si>
+    <t>esmith13laptop</t>
+  </si>
+  <si>
+    <t>C:\E\Dropbox\Lab\[07] Transcription\LivemRNAData</t>
+  </si>
+  <si>
+    <t>C:\E\GitHub\Lab\mRNADynamics</t>
   </si>
 </sst>
 </file>
@@ -315,7 +329,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -350,7 +364,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -559,12 +573,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4725" topLeftCell="J1" activePane="topRight"/>
+      <pane xSplit="4725" topLeftCell="I1" activePane="topRight"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="J8" sqref="J8"/>
+      <selection pane="topRight" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,10 +592,11 @@
     <col min="7" max="7" width="39" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="45.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="50.140625" customWidth="1"/>
+    <col min="10" max="10" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="50.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -610,13 +625,16 @@
         <v>38</v>
       </c>
       <c r="J1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>47</v>
       </c>
@@ -626,9 +644,9 @@
       <c r="H2" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -656,11 +674,11 @@
       <c r="I3" t="s">
         <v>39</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -688,14 +706,14 @@
       <c r="I4" t="s">
         <v>40</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -724,13 +742,16 @@
         <v>54</v>
       </c>
       <c r="J5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" t="s">
         <v>45</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -753,7 +774,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -763,14 +784,14 @@
       <c r="G7" t="s">
         <v>30</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -790,13 +811,16 @@
         <v>41</v>
       </c>
       <c r="J8" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" t="s">
         <v>59</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -815,7 +839,7 @@
       <c r="G9" t="s">
         <v>22</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ComputerFolders update and merge fix
</commit_message>
<xml_diff>
--- a/ComputerFolders.xlsx
+++ b/ComputerFolders.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\E\GitHub\Lab\mRNADynamics\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
@@ -184,9 +179,6 @@
     <t>F:\Eric\Local\[07] Transcription\FISHAnalysisData</t>
   </si>
   <si>
-    <t>F:\Eric\Dropbox\LivemRNAData</t>
-  </si>
-  <si>
     <t>F:\Eric\GitHub\mRNADynamics</t>
   </si>
   <si>
@@ -215,6 +207,9 @@
   </si>
   <si>
     <t>C:\E\GitHub\Lab\mRNADynamics</t>
+  </si>
+  <si>
+    <t>F:\Eric\Dropbox\Lab\[07] Transcription\LivemRNAData</t>
   </si>
 </sst>
 </file>
@@ -329,7 +324,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -364,7 +359,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -576,9 +571,9 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4725" topLeftCell="I1" activePane="topRight"/>
+      <pane xSplit="4725" topLeftCell="G1" activePane="topRight"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="J14" sqref="J14"/>
+      <selection pane="topRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +585,7 @@
     <col min="5" max="5" width="49.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="39" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="47.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="48.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="50.140625" customWidth="1"/>
@@ -625,13 +620,13 @@
         <v>38</v>
       </c>
       <c r="J1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K1" t="s">
         <v>42</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -710,7 +705,7 @@
         <v>44</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -736,19 +731,19 @@
         <v>20</v>
       </c>
       <c r="H5" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="I5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K5" t="s">
         <v>45</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -788,7 +783,7 @@
         <v>45</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -805,19 +800,19 @@
         <v>33</v>
       </c>
       <c r="H8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I8" t="s">
         <v>41</v>
       </c>
       <c r="J8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Unified Database Folder in Dropbox
</commit_message>
<xml_diff>
--- a/ComputerFolders.xlsx
+++ b/ComputerFolders.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
   <si>
     <t>Computer Name</t>
   </si>
@@ -62,9 +62,6 @@
     <t>albert-pc</t>
   </si>
   <si>
-    <t>C:\Users\Albert\Dropbox\LivemRNAData</t>
-  </si>
-  <si>
     <t>phy-steve</t>
   </si>
   <si>
@@ -213,6 +210,21 @@
   </si>
   <si>
     <t>C:\Users\Albert\Dropbox\LivemRNAAlbert</t>
+  </si>
+  <si>
+    <t>C:\Users\albertl\Dropbox\LivemRNADatabase</t>
+  </si>
+  <si>
+    <t>C:\Users\hgarcia\Documents\Dropbox\LivemRNADatabase</t>
+  </si>
+  <si>
+    <t>C:\Users\Albert\Dropbox\LivemRNADatabase</t>
+  </si>
+  <si>
+    <t>C:\users\hgarcia\Documents\Dropbox\LivemRNADatabase</t>
+  </si>
+  <si>
+    <t>C:\Users\hgarcia\Dropbox\LivemRNADatabase</t>
   </si>
 </sst>
 </file>
@@ -574,9 +586,9 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4728" activePane="topRight"/>
-      <selection activeCell="A6" sqref="A6"/>
-      <selection pane="topRight" activeCell="D7" sqref="D7"/>
+      <pane xSplit="4728" topLeftCell="F1" activePane="topRight"/>
+      <selection activeCell="B5" sqref="B5"/>
+      <selection pane="topRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,39 +620,39 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
         <v>46</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>47</v>
-      </c>
-      <c r="H2" t="s">
-        <v>48</v>
       </c>
       <c r="L2" s="2"/>
     </row>
@@ -652,31 +664,31 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -687,34 +699,34 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -722,115 +734,115 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="H5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" t="s">
         <v>62</v>
       </c>
-      <c r="D7" t="s">
-        <v>63</v>
-      </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" t="s">
-        <v>30</v>
-      </c>
       <c r="K8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -844,16 +856,16 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added self to ComputerFolders
</commit_message>
<xml_diff>
--- a/ComputerFolders.xlsx
+++ b/ComputerFolders.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\GregorLab\mRNADynamics\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="48" windowWidth="19440" windowHeight="12240"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
   <si>
     <t>Computer Name</t>
   </si>
@@ -225,6 +230,21 @@
   </si>
   <si>
     <t>C:\Users\hgarcia\Dropbox\LivemRNADatabase</t>
+  </si>
+  <si>
+    <t>fringilla</t>
+  </si>
+  <si>
+    <t>C:\Users\Mark\Dropbox\LivemRNAData</t>
+  </si>
+  <si>
+    <t>C:\Users\Mark\GregorLab\mRNADynamics</t>
+  </si>
+  <si>
+    <t>C:\Users\Mark\GregorLab\Data\FISHAnalysisData</t>
+  </si>
+  <si>
+    <t>C:\Users\Mark\GregorLab\Data\RawData</t>
   </si>
 </sst>
 </file>
@@ -339,7 +359,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -374,7 +394,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -583,30 +603,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4728" topLeftCell="F1" activePane="topRight"/>
+      <pane xSplit="7230" topLeftCell="K1" activePane="topRight"/>
       <selection activeCell="B5" sqref="B5"/>
-      <selection pane="topRight" activeCell="G5" sqref="G5"/>
+      <selection pane="topRight" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="76.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="99.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="99.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="39" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="50.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="48.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="50.109375" customWidth="1"/>
+    <col min="8" max="8" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="50.140625" customWidth="1"/>
+    <col min="12" max="12" width="35.28515625" customWidth="1"/>
+    <col min="13" max="13" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -643,8 +665,11 @@
       <c r="L1" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="M1" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>45</v>
       </c>
@@ -656,7 +681,7 @@
       </c>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -690,8 +715,11 @@
       <c r="K3" t="s">
         <v>41</v>
       </c>
+      <c r="M3" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -728,8 +756,11 @@
       <c r="L4" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="M4" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -766,8 +797,11 @@
       <c r="L5" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="M5" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -782,7 +816,7 @@
       </c>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -799,7 +833,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -816,7 +850,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -844,8 +878,11 @@
       <c r="L9" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="M9" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -885,7 +922,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -902,7 +939,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Added JB on phy-TGLAB11 to folders
</commit_message>
<xml_diff>
--- a/ComputerFolders.xlsx
+++ b/ComputerFolders.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\GregorLab\mRNADynamics\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="76">
   <si>
     <t>Computer Name</t>
   </si>
@@ -245,6 +240,15 @@
   </si>
   <si>
     <t>C:\Users\Mark\GregorLab\Data\RawData</t>
+  </si>
+  <si>
+    <t>bothma</t>
+  </si>
+  <si>
+    <t>C:\Users\bothma\Dropbox\LivemRNADatabase</t>
+  </si>
+  <si>
+    <t>C:\Users\bothma\Dropbox\LivemRNAData</t>
   </si>
 </sst>
 </file>
@@ -359,7 +363,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -394,7 +398,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -603,12 +607,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7230" topLeftCell="K1" activePane="topRight"/>
+      <pane xSplit="2040" topLeftCell="L1" activePane="topRight"/>
       <selection activeCell="B5" sqref="B5"/>
-      <selection pane="topRight" activeCell="M3" sqref="M3"/>
+      <selection pane="topRight" activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,7 +632,7 @@
     <col min="13" max="13" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -668,8 +672,11 @@
       <c r="M1" t="s">
         <v>68</v>
       </c>
+      <c r="N1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>45</v>
       </c>
@@ -680,8 +687,11 @@
         <v>47</v>
       </c>
       <c r="L2" s="2"/>
+      <c r="N2" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -718,8 +728,11 @@
       <c r="M3" t="s">
         <v>72</v>
       </c>
+      <c r="N3" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -759,8 +772,11 @@
       <c r="M4" t="s">
         <v>71</v>
       </c>
+      <c r="N4" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -800,8 +816,11 @@
       <c r="M5" t="s">
         <v>69</v>
       </c>
+      <c r="N5" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -815,8 +834,11 @@
         <v>19</v>
       </c>
       <c r="L6" s="2"/>
+      <c r="N6" t="s">
+        <v>75</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -833,7 +855,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -849,8 +871,11 @@
       <c r="L8" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="N8" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -881,8 +906,11 @@
       <c r="M9" t="s">
         <v>70</v>
       </c>
+      <c r="N9" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -903,6 +931,9 @@
       </c>
       <c r="K10" t="s">
         <v>44</v>
+      </c>
+      <c r="N10" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added step to find pixel size
Hack for data from Princeton confocal, just set to 220nm. Xresolution
field has same value of 72 inches (?) for images of different
magnifications.
</commit_message>
<xml_diff>
--- a/ComputerFolders.xlsx
+++ b/ComputerFolders.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\E\GitHub\Lab\mRNADynamics\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="15600" windowHeight="11760"/>
   </bookViews>
@@ -16,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -151,9 +146,6 @@
     <t>bothma-desktop</t>
   </si>
   <si>
-    <t>D:\MS2LiveImaging\SourcePath</t>
-  </si>
-  <si>
     <t>D:\MS2LiveImaging\Code\MS2Pausing\FISHCode</t>
   </si>
   <si>
@@ -278,6 +270,9 @@
   </si>
   <si>
     <t>esmith11desktop</t>
+  </si>
+  <si>
+    <t>G:\liveImaging</t>
   </si>
 </sst>
 </file>
@@ -392,7 +387,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -427,7 +422,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -639,9 +634,9 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="7245" topLeftCell="K1" activePane="topRight"/>
+      <pane xSplit="7245" topLeftCell="L1" activePane="topRight"/>
       <selection activeCell="A9" sqref="A9"/>
-      <selection pane="topRight" activeCell="K1" sqref="K1"/>
+      <selection pane="topRight" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,19 +688,19 @@
         <v>37</v>
       </c>
       <c r="J1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L1" t="s">
         <v>40</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O1" t="s">
         <v>20</v>
@@ -716,20 +711,20 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
         <v>45</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>46</v>
-      </c>
-      <c r="H2" t="s">
-        <v>47</v>
       </c>
       <c r="M2" s="2"/>
       <c r="O2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -755,7 +750,7 @@
         <v>26</v>
       </c>
       <c r="H3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I3" t="s">
         <v>38</v>
@@ -767,16 +762,16 @@
         <v>38</v>
       </c>
       <c r="L3" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="N3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O3" t="s">
         <v>26</v>
       </c>
       <c r="P3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -802,7 +797,7 @@
         <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I4" t="s">
         <v>39</v>
@@ -814,19 +809,19 @@
         <v>39</v>
       </c>
       <c r="L4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O4" t="s">
         <v>27</v>
       </c>
       <c r="P4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -834,54 +829,54 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
         <v>63</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>64</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>65</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>66</v>
       </c>
-      <c r="F5" t="s">
-        <v>67</v>
-      </c>
       <c r="G5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="P5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -894,7 +889,7 @@
       </c>
       <c r="M6" s="2"/>
       <c r="O6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -902,10 +897,10 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" t="s">
         <v>61</v>
-      </c>
-      <c r="D7" t="s">
-        <v>62</v>
       </c>
       <c r="E7" t="s">
         <v>16</v>
@@ -925,16 +920,16 @@
         <v>29</v>
       </c>
       <c r="L8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -951,31 +946,31 @@
         <v>32</v>
       </c>
       <c r="H9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O9" t="s">
         <v>32</v>
       </c>
       <c r="P9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -998,7 +993,7 @@
         <v>21</v>
       </c>
       <c r="L10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O10" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Enabling Lattice Light Sheet data import
various Lattice-specific functions to flatfield correct and export
images to Raw Data.
Additionally, introduced Heinrichs folders to the xls
</commit_message>
<xml_diff>
--- a/ComputerFolders.xlsx
+++ b/ComputerFolders.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hernan\Documents\My Papers\LivemRNA\mRNADynamics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TGlab\mRNADynamics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="3060" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="1260" yWindow="3060" windowWidth="25605" windowHeight="16065"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="117">
   <si>
     <t>Computer Name</t>
   </si>
@@ -350,6 +350,33 @@
   </si>
   <si>
     <t>D:\Hernan\Dropbox\LivemRNAData</t>
+  </si>
+  <si>
+    <t>hgsasu</t>
+  </si>
+  <si>
+    <t>Grabmayr</t>
+  </si>
+  <si>
+    <t>D:\Tglab\LivemRNA\RawData</t>
+  </si>
+  <si>
+    <t>D:\Tglab\LivemRNA\AnalysisData</t>
+  </si>
+  <si>
+    <t>C:\Users\Grabmayr\Dropbox\LivemRNADatabaseHepG</t>
+  </si>
+  <si>
+    <t>C:\Users\Grabmayr\Dropbox\LivemRNAAlbert</t>
+  </si>
+  <si>
+    <t>C:\Users\Grabmayr\Dropbox\LivemRNAHeinrich</t>
+  </si>
+  <si>
+    <t>DropboxHeinrich</t>
+  </si>
+  <si>
+    <t>D:\TGlab\mRNADynamics</t>
   </si>
 </sst>
 </file>
@@ -732,36 +759,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B16" sqref="B16:B28"/>
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="76.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="76.81640625" customWidth="1"/>
-    <col min="5" max="5" width="99.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="76.85546875" customWidth="1"/>
+    <col min="5" max="5" width="99.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="39" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="50.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="50.453125" customWidth="1"/>
-    <col min="11" max="11" width="47.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="50.1796875" customWidth="1"/>
-    <col min="14" max="14" width="35.36328125" customWidth="1"/>
-    <col min="15" max="15" width="45.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="43.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.1796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="38.81640625" customWidth="1"/>
+    <col min="9" max="9" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="50.42578125" customWidth="1"/>
+    <col min="11" max="11" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="50.140625" customWidth="1"/>
+    <col min="14" max="14" width="35.42578125" customWidth="1"/>
+    <col min="15" max="15" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="38.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -816,8 +843,11 @@
       <c r="R1" t="s">
         <v>84</v>
       </c>
+      <c r="S1" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
@@ -837,8 +867,11 @@
       <c r="R2" t="s">
         <v>83</v>
       </c>
+      <c r="S2" t="s">
+        <v>109</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -890,8 +923,11 @@
       <c r="R3" t="s">
         <v>80</v>
       </c>
+      <c r="S3" t="s">
+        <v>110</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -946,8 +982,11 @@
       <c r="R4" t="s">
         <v>85</v>
       </c>
+      <c r="S4" t="s">
+        <v>111</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1002,8 +1041,11 @@
       <c r="R5" t="s">
         <v>81</v>
       </c>
+      <c r="S5" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1024,7 +1066,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1046,8 +1088,11 @@
       <c r="G7" t="s">
         <v>17</v>
       </c>
+      <c r="S7" t="s">
+        <v>113</v>
+      </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1076,7 +1121,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -1096,83 +1141,98 @@
         <v>90</v>
       </c>
       <c r="N9" s="2"/>
+      <c r="S9" t="s">
+        <v>114</v>
+      </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>115</v>
+      </c>
+      <c r="N10" s="2"/>
+      <c r="S10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>105</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>30</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>92</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>33</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H11" t="s">
         <v>29</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I11" t="s">
         <v>42</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J11" t="s">
         <v>49</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K11" t="s">
         <v>49</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L11" t="s">
         <v>49</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M11" t="s">
         <v>47</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="N11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="O10" t="s">
+      <c r="O11" t="s">
         <v>58</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P11" t="s">
         <v>29</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q11" t="s">
         <v>68</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R11" t="s">
         <v>82</v>
       </c>
+      <c r="S11" t="s">
+        <v>116</v>
+      </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>91</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" t="s">
         <v>15</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G12" t="s">
         <v>19</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H12" t="s">
         <v>19</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M12" t="s">
         <v>38</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1193,7 +1253,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1210,7 +1270,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
More fixes to handle two-color-spot data
</commit_message>
<xml_diff>
--- a/ComputerFolders.xlsx
+++ b/ComputerFolders.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TGlab\mRNADynamics\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="3060" windowWidth="25605" windowHeight="16065"/>
+    <workbookView xWindow="1260" yWindow="3060" windowWidth="20640" windowHeight="13440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="118">
   <si>
     <t>Computer Name</t>
   </si>
@@ -377,6 +372,9 @@
   </si>
   <si>
     <t>D:\TGlab\mRNADynamics</t>
+  </si>
+  <si>
+    <t>C:\Users\hgarcia\Dropbox\LivemRNAAlbert</t>
   </si>
 </sst>
 </file>
@@ -515,7 +513,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -550,7 +548,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -762,8 +760,8 @@
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S12" sqref="S12"/>
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,6 +1085,9 @@
       </c>
       <c r="G7" t="s">
         <v>17</v>
+      </c>
+      <c r="H7" t="s">
+        <v>117</v>
       </c>
       <c r="S7" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
added myself to computer folders
</commit_message>
<xml_diff>
--- a/ComputerFolders.xlsx
+++ b/ComputerFolders.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ArmandoReimer\Documents\MATLAB\mRNADynamics\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="3060" windowWidth="20640" windowHeight="13440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="130">
   <si>
     <t>Computer Name</t>
   </si>
@@ -398,6 +393,24 @@
   </si>
   <si>
     <t>ArmandoReimer</t>
+  </si>
+  <si>
+    <t>inka-mac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Users/inka/Documents/PrincetonJP/RawData </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Users/inka/Documents/PrincetonJP/FishToolbox </t>
+  </si>
+  <si>
+    <t>inkab</t>
+  </si>
+  <si>
+    <t>/Users/inka/Dropbox/LivemRNADatabase</t>
+  </si>
+  <si>
+    <t>/Users/inka/Documents/PrincetonJP/mRNADynamics</t>
   </si>
 </sst>
 </file>
@@ -539,7 +552,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -574,7 +587,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -783,39 +796,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U3" sqref="U3"/>
+      <selection pane="topRight" activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="76.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="76.85546875" customWidth="1"/>
-    <col min="5" max="5" width="99.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="76.83203125" customWidth="1"/>
+    <col min="5" max="5" width="99.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="39" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="50.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="50.42578125" customWidth="1"/>
-    <col min="11" max="11" width="47.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="50.140625" customWidth="1"/>
-    <col min="14" max="14" width="35.42578125" customWidth="1"/>
-    <col min="15" max="15" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="38.85546875" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" customWidth="1"/>
-    <col min="20" max="20" width="36.28515625" style="3" customWidth="1"/>
-    <col min="21" max="21" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="50.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="50.5" customWidth="1"/>
+    <col min="11" max="11" width="47.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="50.1640625" customWidth="1"/>
+    <col min="14" max="14" width="35.5" customWidth="1"/>
+    <col min="15" max="15" width="45.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="43.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="38.83203125" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" customWidth="1"/>
+    <col min="20" max="20" width="36.33203125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -876,8 +889,11 @@
       <c r="T1" s="3" t="s">
         <v>118</v>
       </c>
+      <c r="U1" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21">
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
@@ -903,8 +919,11 @@
       <c r="T2" s="3" t="s">
         <v>123</v>
       </c>
+      <c r="U2" t="s">
+        <v>127</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="28">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -962,8 +981,11 @@
       <c r="T3" s="3" t="s">
         <v>120</v>
       </c>
+      <c r="U3" t="s">
+        <v>125</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="28">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1024,8 +1046,11 @@
       <c r="T4" s="3" t="s">
         <v>121</v>
       </c>
+      <c r="U4" t="s">
+        <v>126</v>
+      </c>
     </row>
-    <row r="5" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="28">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1086,8 +1111,11 @@
       <c r="T5" s="3" t="s">
         <v>122</v>
       </c>
+      <c r="U5" t="s">
+        <v>128</v>
+      </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1108,7 +1136,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1137,7 +1165,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1166,7 +1194,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -1190,7 +1218,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -1199,7 +1227,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="28">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1254,8 +1282,11 @@
       <c r="T11" s="3" t="s">
         <v>119</v>
       </c>
+      <c r="U11" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1301,7 +1332,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1318,7 +1349,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
added a case for my computer
</commit_message>
<xml_diff>
--- a/ComputerFolders.xlsx
+++ b/ComputerFolders.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="132">
   <si>
     <t>Computer Name</t>
   </si>
@@ -411,6 +411,12 @@
   </si>
   <si>
     <t>/Users/inka/Documents/PrincetonJP/mRNADynamics</t>
+  </si>
+  <si>
+    <t>DropboxEmilia</t>
+  </si>
+  <si>
+    <t>/Users/inka/Dropbox/LivemRNAEmilia</t>
   </si>
 </sst>
 </file>
@@ -474,8 +480,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -489,11 +501,17 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -796,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
@@ -1227,91 +1245,99 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="28">
+    <row r="11" spans="1:21">
       <c r="A11" t="s">
+        <v>130</v>
+      </c>
+      <c r="U11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="28">
+      <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>105</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>30</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>92</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>33</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H12" t="s">
         <v>29</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I12" t="s">
         <v>42</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J12" t="s">
         <v>49</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K12" t="s">
         <v>49</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L12" t="s">
         <v>49</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M12" t="s">
         <v>47</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="N12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O12" t="s">
         <v>58</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P12" t="s">
         <v>29</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="Q12" t="s">
         <v>68</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R12" t="s">
         <v>82</v>
       </c>
-      <c r="S11" t="s">
+      <c r="S12" t="s">
         <v>116</v>
       </c>
-      <c r="T11" s="3" t="s">
+      <c r="T12" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="U11" t="s">
+      <c r="U12" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
-      <c r="A12" t="s">
+    <row r="13" spans="1:21">
+      <c r="A13" t="s">
         <v>7</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>9</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>91</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" t="s">
         <v>15</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>19</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H13" t="s">
         <v>19</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M13" t="s">
         <v>38</v>
       </c>
-      <c r="P12" t="s">
+      <c r="P13" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added row to computerfolders xls
</commit_message>
<xml_diff>
--- a/ComputerFolders.xlsx
+++ b/ComputerFolders.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14220"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="133">
   <si>
     <t>Computer Name</t>
   </si>
@@ -417,6 +417,9 @@
   </si>
   <si>
     <t>/Users/inka/Dropbox/LivemRNAEmilia</t>
+  </si>
+  <si>
+    <t>C:\Users\Albert\Dropbox\LivemRNAEmilia</t>
   </si>
 </sst>
 </file>
@@ -817,36 +820,36 @@
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U11" sqref="U11"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="76.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="76.83203125" customWidth="1"/>
-    <col min="5" max="5" width="99.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="76.77734375" customWidth="1"/>
+    <col min="5" max="5" width="99.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="39" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="50.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="50.5" customWidth="1"/>
-    <col min="11" max="11" width="47.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="50.1640625" customWidth="1"/>
-    <col min="14" max="14" width="35.5" customWidth="1"/>
-    <col min="15" max="15" width="45.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="43.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="38.83203125" customWidth="1"/>
+    <col min="9" max="9" width="50.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="50.44140625" customWidth="1"/>
+    <col min="11" max="11" width="47.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="50.109375" customWidth="1"/>
+    <col min="14" max="14" width="35.44140625" customWidth="1"/>
+    <col min="15" max="15" width="45.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="43.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="38.77734375" customWidth="1"/>
     <col min="19" max="19" width="12.33203125" customWidth="1"/>
     <col min="20" max="20" width="36.33203125" style="3" customWidth="1"/>
     <col min="21" max="21" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -911,7 +914,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
@@ -941,7 +944,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="28">
+    <row r="3" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1003,7 +1006,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="28">
+    <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1068,7 +1071,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="28">
+    <row r="5" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1133,7 +1136,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1154,7 +1157,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1183,7 +1186,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1212,7 +1215,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -1236,7 +1239,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -1245,15 +1248,18 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>130</v>
       </c>
+      <c r="E11" t="s">
+        <v>132</v>
+      </c>
       <c r="U11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="28">
+    <row r="12" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1312,7 +1318,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1358,7 +1364,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1375,7 +1381,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Added function to checkparticletracking
hit '\' and click particle to move to that particle
</commit_message>
<xml_diff>
--- a/ComputerFolders.xlsx
+++ b/ComputerFolders.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="3060" windowWidth="20640" windowHeight="13440"/>
+    <workbookView xWindow="1260" yWindow="3060" windowWidth="20640" windowHeight="6675"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -786,8 +786,8 @@
   <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U3" sqref="U3"/>
+      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,8 +810,8 @@
     <col min="16" max="16" width="43.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="38.85546875" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" customWidth="1"/>
-    <col min="20" max="20" width="36.28515625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="52.85546875" customWidth="1"/>
+    <col min="20" max="20" width="56" style="3" customWidth="1"/>
     <col min="21" max="21" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
ComputerFolders: moving my data
</commit_message>
<xml_diff>
--- a/ComputerFolders.xlsx
+++ b/ComputerFolders.xlsx
@@ -149,9 +149,6 @@
     <t>emsthree</t>
   </si>
   <si>
-    <t>F:\Eric\GitHub\mRNADynamics</t>
-  </si>
-  <si>
     <t>jacquess-macbook-pro.local</t>
   </si>
   <si>
@@ -254,15 +251,6 @@
     <t>C:\E\Dropbox\Lab\07_Transcription\LivemRNAData</t>
   </si>
   <si>
-    <t>F:\Eric\Local\07_Transcription\RawData</t>
-  </si>
-  <si>
-    <t>F:\Eric\Local\07_Transcription\FISHAnalysisData</t>
-  </si>
-  <si>
-    <t>F:\Eric\Dropbox\Lab\07_Transcription\LivemRNAData</t>
-  </si>
-  <si>
     <t>/Volumes/Data/RawMs2movie</t>
   </si>
   <si>
@@ -435,6 +423,18 @@
   </si>
   <si>
     <t>F:\Net\GitHub\mRNADynamics</t>
+  </si>
+  <si>
+    <t>E:\Eric\Local\07_Transcription\RawData</t>
+  </si>
+  <si>
+    <t>E:\Eric\Local\07_Transcription\FISHAnalysisData</t>
+  </si>
+  <si>
+    <t>E:\Eric\Dropbox\Lab\07_Transcription\LivemRNAData</t>
+  </si>
+  <si>
+    <t>E:\Eric\GitHub\mRNADynamics</t>
   </si>
 </sst>
 </file>
@@ -835,8 +835,8 @@
   <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V14" sqref="V14"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,7 +875,7 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
@@ -896,19 +896,19 @@
         <v>34</v>
       </c>
       <c r="K1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M1" t="s">
         <v>35</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P1" t="s">
         <v>18</v>
@@ -917,16 +917,16 @@
         <v>18</v>
       </c>
       <c r="R1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="S1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="U1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="V1" t="s">
         <v>18</v>
@@ -944,25 +944,25 @@
       </c>
       <c r="N2" s="2"/>
       <c r="P2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="S2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="T2" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="U2" t="s">
         <v>123</v>
       </c>
-      <c r="U2" t="s">
-        <v>127</v>
-      </c>
       <c r="V2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="28.9" x14ac:dyDescent="0.3">
@@ -970,13 +970,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E3" t="s">
         <v>31</v>
@@ -991,43 +991,43 @@
         <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>77</v>
+        <v>134</v>
       </c>
       <c r="J3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P3" t="s">
         <v>23</v>
       </c>
       <c r="Q3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="R3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="S3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="U3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="V3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="28.9" x14ac:dyDescent="0.3">
@@ -1035,13 +1035,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E4" t="s">
         <v>32</v>
@@ -1056,46 +1056,46 @@
         <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>135</v>
       </c>
       <c r="J4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M4" t="s">
         <v>36</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P4" t="s">
         <v>24</v>
       </c>
       <c r="Q4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="R4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="S4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="U4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="V4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="28.9" x14ac:dyDescent="0.3">
@@ -1103,88 +1103,88 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" t="s">
         <v>53</v>
       </c>
-      <c r="D5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>54</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>55</v>
       </c>
-      <c r="G5" t="s">
-        <v>56</v>
-      </c>
       <c r="H5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I5" t="s">
-        <v>79</v>
+        <v>136</v>
       </c>
       <c r="J5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="R5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="S5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="U5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="V5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H6" t="s">
         <v>17</v>
       </c>
       <c r="N6" s="2"/>
       <c r="P6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
@@ -1192,16 +1192,16 @@
         <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" t="s">
         <v>51</v>
-      </c>
-      <c r="D7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E7" t="s">
-        <v>52</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
@@ -1210,10 +1210,10 @@
         <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="S7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
@@ -1221,13 +1221,13 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H8" t="s">
         <v>26</v>
@@ -1236,10 +1236,10 @@
         <v>37</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P8" t="s">
         <v>37</v>
@@ -1247,46 +1247,46 @@
     </row>
     <row r="9" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="N9" s="2"/>
       <c r="S9" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="N10" s="2"/>
       <c r="S10" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E11" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="U11" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="28.9" x14ac:dyDescent="0.3">
@@ -1294,13 +1294,13 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C12" t="s">
         <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E12" t="s">
         <v>33</v>
@@ -1309,46 +1309,46 @@
         <v>29</v>
       </c>
       <c r="I12" t="s">
-        <v>42</v>
+        <v>137</v>
       </c>
       <c r="J12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P12" t="s">
         <v>29</v>
       </c>
       <c r="Q12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="R12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="S12" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="T12" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="U12" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="V12" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
@@ -1362,7 +1362,7 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F13" t="s">
         <v>15</v>

</xml_diff>